<commit_message>
oracle database에서 raw_data 받아와서 저per전략 성과 class로 구현 완료
</commit_message>
<xml_diff>
--- a/Make csv/계정 설명.xlsx
+++ b/Make csv/계정 설명.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SH-NoteBook\Google 드라이브\KSIF (1)\GIT\Make csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SH-NoteBook\Google 드라이브\KSIF\GIT\Make csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>자본총계</t>
   </si>
@@ -285,13 +285,23 @@
   <si>
     <t>아나 이거 NR.FQ1로 받음</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직전 4분기 총합을 이용하려면 이걸로 받아야함.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M115020.M</t>
+  </si>
+  <si>
+    <t>자본총계(지배)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,8 +326,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,8 +356,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -339,13 +371,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3664FD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3664FD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -362,14 +412,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -644,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -693,255 +786,287 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="B4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B7" s="1" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B11" s="1" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:5" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="29" spans="1:5" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B29" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B33" s="1" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B36" s="1" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B39" s="1" t="s">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B42" s="1" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>59</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B45" s="1" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D46" s="4" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="D48" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>62</v>
-      </c>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>